<commit_message>
update validator script to update the references to relative
</commit_message>
<xml_diff>
--- a/Validate_File/test_resources.xlsx
+++ b/Validate_File/test_resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/Validate_File/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C2E040-4186-C24A-BD26-6780066387D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47246BF1-0330-3343-BB99-D5DC4C702B6E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{C41D9D53-C301-DE45-AC77-254FFD7F4D5F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>ehoN2kZnYuW5z0Di4Kkno5w3,eiSX3g2gt4tJIs7-6h7nJjA3,e1Jw-ETrL1kZAPiXl3uSMWw3,eZAjx5sRd6AgpTlKjDh4b5w3,ejPvGuBUqYJkCweOPRabvYg3</t>
+  </si>
+  <si>
+    <t>e4W4rmGe9QzuGm2Dy4NBqVc0KDe6yGld6HW95UuN-Qd03</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3411C30-C3C7-5747-9BA0-310370083C22}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -499,6 +505,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>